<commit_message>
jeden dodany wiersz bbb
</commit_message>
<xml_diff>
--- a/ang.xlsx
+++ b/ang.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>reproducible</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>surowy/czysty</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>bbbb</t>
   </si>
 </sst>
 </file>
@@ -439,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,6 +573,14 @@
       </c>
       <c r="B17" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>